<commit_message>
[AS]- Updated PEF-INT 3.2 Change Details sheet
</commit_message>
<xml_diff>
--- a/REF-INT 3.2 Change Details.xlsx
+++ b/REF-INT 3.2 Change Details.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cts1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SOAP-GIT\BMV_SOAP_PACKS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="74">
   <si>
     <t>S.No.</t>
   </si>
@@ -156,6 +156,105 @@
   </si>
   <si>
     <t xml:space="preserve">We have to disable all the testcases </t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_1_ValidationTest</t>
+  </si>
+  <si>
+    <t>searchOnlineAccount_1_0148</t>
+  </si>
+  <si>
+    <t>searchOnlineAccount_1_0149</t>
+  </si>
+  <si>
+    <t>UserDetailsPS</t>
+  </si>
+  <si>
+    <t>UpdateAddress</t>
+  </si>
+  <si>
+    <t>updateAddress_007</t>
+  </si>
+  <si>
+    <t>OTLC-1006</t>
+  </si>
+  <si>
+    <t>As per the analysis, Address field validation is handled at MyO2 end which is a consumer for MUD service, SO there will not be any scenario where empty address fields will come to SOA in 3.2. In 3.1 this validation is not there because of that it is working fine.</t>
+  </si>
+  <si>
+    <t>SearchCriteria_BySearchCriteriaType</t>
+  </si>
+  <si>
+    <t>001. SearchCriteria by CustNum</t>
+  </si>
+  <si>
+    <t>OTLC-1239</t>
+  </si>
+  <si>
+    <t>CustNum changed, record not present in LeanCRM (Because of migration)</t>
+  </si>
+  <si>
+    <t>As per discussion on 08/30 with offshore team and comments given by Nitish on OTLC-1239, changed data in test cases</t>
+  </si>
+  <si>
+    <t>003. SeachCriteria by portalID</t>
+  </si>
+  <si>
+    <t>portalId changed, record not present in LeanCRM (Because of migration)</t>
+  </si>
+  <si>
+    <t>008. SeachCriteria by UID</t>
+  </si>
+  <si>
+    <t>UID changed, record not present in LeanCRM (Because of migration)</t>
+  </si>
+  <si>
+    <t>009. SeachCriteria by BFID</t>
+  </si>
+  <si>
+    <t>BFID changed, record not present in LeanCRM (Because of migration)</t>
+  </si>
+  <si>
+    <t>002. SearchCriteria by MSISDN + Summary</t>
+  </si>
+  <si>
+    <t>MSISDN changed, record not present in LeanCRM (Because of migration)</t>
+  </si>
+  <si>
+    <t>SearchOption_BySearchOption_SUMMARY</t>
+  </si>
+  <si>
+    <t>036. SearchCriteria by MSISDN + Summary</t>
+  </si>
+  <si>
+    <t>SearchOption_BySearchOption_ALL</t>
+  </si>
+  <si>
+    <t>045. SearchCriteria by MSISDN + All</t>
+  </si>
+  <si>
+    <t>SearchOption_BySearchOption_ResultSpecific_LegacyAandRCustomerInfo</t>
+  </si>
+  <si>
+    <t>054. SearchCriteria by MSISDN + legacyAandRCustomerInfo</t>
+  </si>
+  <si>
+    <t>SearchOption_BySearchOption_ResultSpecific_portalInfo</t>
+  </si>
+  <si>
+    <t>063. SearchCriteria by MSISDN + potalinfo</t>
+  </si>
+  <si>
+    <t>SearchOption_BySearchOption_ResultSpecific_accountLinkageInfo</t>
+  </si>
+  <si>
+    <t>090. SearchCriteria by MSISDN + accountLinkageInfo</t>
+  </si>
+  <si>
+    <t>SearchOption_BySearchOption_PORTAL</t>
+  </si>
+  <si>
+    <t>099. SearchCriteria by MSISDN + SUMMARY</t>
   </si>
 </sst>
 </file>
@@ -193,7 +292,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -216,19 +315,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -236,6 +366,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -545,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,304 +736,781 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="180" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="4"/>
+      <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="4"/>
+      <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="4"/>
+      <c r="I9" s="2"/>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>15</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>16</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>17</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="5"/>
+    </row>
+    <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="7"/>
+      <c r="F23" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" s="7"/>
+      <c r="F27" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E28" s="7"/>
+      <c r="F28" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="7"/>
+      <c r="F29" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" s="7"/>
+      <c r="F30" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E31" s="7"/>
+      <c r="F31" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" s="7"/>
+      <c r="F32" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" s="7"/>
+      <c r="F33" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>33</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>34</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" s="8"/>
+      <c r="F35" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="G14:G35"/>
+    <mergeCell ref="H14:H35"/>
+    <mergeCell ref="E14:E35"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
[AS]-Updated UAS.SearchOnlineAccount1&2 ans Change Details sheet
</commit_message>
<xml_diff>
--- a/REF-INT 3.2 Change Details.xlsx
+++ b/REF-INT 3.2 Change Details.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="89">
   <si>
     <t>S.No.</t>
   </si>
@@ -255,6 +255,51 @@
   </si>
   <si>
     <t>099. SearchCriteria by MSISDN + SUMMARY</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_1_013</t>
+  </si>
+  <si>
+    <t>SearchCriteria_ByMultipleSearchCriteriaType</t>
+  </si>
+  <si>
+    <t>Need to uncomment the portalOrIdentitySwitch from the testcase for 3.2</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_1_0037</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_1_0046</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_1_0064</t>
+  </si>
+  <si>
+    <t>SearchOption_BySearchOption_ResultSpecific_billingInfo</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_1_0091</t>
+  </si>
+  <si>
+    <t>searchOnlineAccount_2_013</t>
+  </si>
+  <si>
+    <t>searchOnlineAccount_2_0037</t>
+  </si>
+  <si>
+    <t>searchOnlineAccount_2_0046</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_2_0055</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_2_0064</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_2_0073</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_2_0091</t>
   </si>
 </sst>
 </file>
@@ -356,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -367,14 +412,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -382,6 +427,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -690,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B41" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42:I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,472 +1096,822 @@
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>13</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="5" t="s">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I14" s="5"/>
+      <c r="I14" s="4"/>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="5" t="s">
+      <c r="B15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>54</v>
       </c>
       <c r="E15" s="7"/>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="4" t="s">
         <v>55</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
-      <c r="I15" s="5"/>
+      <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="5" t="s">
+      <c r="B16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>56</v>
       </c>
       <c r="E16" s="7"/>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="4" t="s">
         <v>57</v>
       </c>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
-      <c r="I16" s="5"/>
+      <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="A17" s="4">
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="B17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>58</v>
       </c>
       <c r="E17" s="7"/>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="4" t="s">
         <v>59</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
-      <c r="I17" s="5"/>
+      <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="B18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E18" s="7"/>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
-      <c r="I18" s="5"/>
+      <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="A19" s="4">
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="5" t="s">
+      <c r="B19" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>63</v>
       </c>
       <c r="E19" s="7"/>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
-      <c r="I19" s="5"/>
+      <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
-        <v>19</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>65</v>
       </c>
       <c r="E20" s="7"/>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
-      <c r="I20" s="5"/>
+      <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+      <c r="A21" s="4">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="6" t="s">
+      <c r="B21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>67</v>
       </c>
       <c r="E21" s="7"/>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
-      <c r="I21" s="5"/>
+      <c r="I21" s="4"/>
     </row>
     <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+      <c r="A22" s="4">
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="6" t="s">
+      <c r="B22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>69</v>
       </c>
       <c r="E22" s="7"/>
-      <c r="F22" s="5" t="s">
+      <c r="F22" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
-      <c r="I22" s="5"/>
+      <c r="I22" s="4"/>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
+      <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="6" t="s">
+      <c r="B23" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>71</v>
       </c>
       <c r="E23" s="7"/>
-      <c r="F23" s="5" t="s">
+      <c r="F23" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
-      <c r="I23" s="5"/>
+      <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+      <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="6" t="s">
+      <c r="B24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>73</v>
       </c>
       <c r="E24" s="7"/>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
-      <c r="I24" s="5"/>
+      <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+      <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" s="5" t="s">
+      <c r="B25" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>50</v>
       </c>
       <c r="E25" s="7"/>
-      <c r="F25" s="5" t="s">
+      <c r="F25" s="4" t="s">
         <v>52</v>
       </c>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
-      <c r="I25" s="5"/>
+      <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="A26" s="4">
         <v>25</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="5" t="s">
+      <c r="B26" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>54</v>
       </c>
       <c r="E26" s="7"/>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="4" t="s">
         <v>55</v>
       </c>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
-      <c r="I26" s="5"/>
+      <c r="I26" s="4"/>
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+      <c r="A27" s="4">
         <v>26</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="5" t="s">
+      <c r="B27" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>56</v>
       </c>
       <c r="E27" s="7"/>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="4" t="s">
         <v>57</v>
       </c>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
-      <c r="I27" s="5"/>
+      <c r="I27" s="4"/>
     </row>
     <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="A28" s="4">
         <v>27</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="5" t="s">
+      <c r="B28" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="4" t="s">
         <v>58</v>
       </c>
       <c r="E28" s="7"/>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="4" t="s">
         <v>59</v>
       </c>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
-      <c r="I28" s="5"/>
+      <c r="I28" s="4"/>
     </row>
     <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
+      <c r="A29" s="4">
         <v>28</v>
       </c>
-      <c r="B29" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" s="5" t="s">
+      <c r="B29" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>60</v>
       </c>
       <c r="E29" s="7"/>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
-      <c r="I29" s="5"/>
+      <c r="I29" s="4"/>
     </row>
     <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+      <c r="A30" s="4">
         <v>29</v>
       </c>
-      <c r="B30" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="5" t="s">
+      <c r="B30" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>63</v>
       </c>
       <c r="E30" s="7"/>
-      <c r="F30" s="5" t="s">
+      <c r="F30" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
-      <c r="I30" s="5"/>
+      <c r="I30" s="4"/>
     </row>
     <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
+      <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="B31" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="5" t="s">
+      <c r="B31" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>65</v>
       </c>
       <c r="E31" s="7"/>
-      <c r="F31" s="5" t="s">
+      <c r="F31" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
-      <c r="I31" s="5"/>
+      <c r="I31" s="4"/>
     </row>
     <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
+      <c r="A32" s="4">
         <v>31</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="6" t="s">
+      <c r="B32" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="4" t="s">
         <v>67</v>
       </c>
       <c r="E32" s="7"/>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
-      <c r="I32" s="5"/>
+      <c r="I32" s="4"/>
     </row>
     <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
+      <c r="A33" s="4">
         <v>32</v>
       </c>
-      <c r="B33" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" s="6" t="s">
+      <c r="B33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="4" t="s">
         <v>69</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="5" t="s">
+      <c r="F33" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
-      <c r="I33" s="5"/>
+      <c r="I33" s="4"/>
     </row>
     <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
+      <c r="A34" s="4">
         <v>33</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="6" t="s">
+      <c r="B34" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="4" t="s">
         <v>71</v>
       </c>
       <c r="E34" s="7"/>
-      <c r="F34" s="5" t="s">
+      <c r="F34" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
-      <c r="I34" s="5"/>
+      <c r="I34" s="4"/>
     </row>
     <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
+      <c r="A35" s="4">
         <v>34</v>
       </c>
-      <c r="B35" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="6" t="s">
+      <c r="B35" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="4" t="s">
         <v>73</v>
       </c>
       <c r="E35" s="8"/>
-      <c r="F35" s="5" t="s">
+      <c r="F35" s="4" t="s">
         <v>61</v>
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="8"/>
-      <c r="I35" s="5"/>
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>35</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+    </row>
+    <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>36</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+    </row>
+    <row r="38" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>37</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+    </row>
+    <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>38</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+    </row>
+    <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>39</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+    </row>
+    <row r="41" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>40</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+    </row>
+    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>41</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+    </row>
+    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>42</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+    </row>
+    <row r="44" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>43</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+    </row>
+    <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>44</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E45" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+    </row>
+    <row r="46" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>45</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+    </row>
+    <row r="47" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>46</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+    </row>
+    <row r="48" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>47</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+    </row>
+    <row r="49" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="4">
+        <v>48</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D49" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
[AS]-Updated UAS operations for OTLC-1234 and change details sheet
</commit_message>
<xml_diff>
--- a/REF-INT 3.2 Change Details.xlsx
+++ b/REF-INT 3.2 Change Details.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="252"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="112">
   <si>
     <t>S.No.</t>
   </si>
@@ -300,6 +300,75 @@
   </si>
   <si>
     <t>searchOnlineAccounts_2_0091</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_1_0024</t>
+  </si>
+  <si>
+    <t>SearchCriteria_BySearchCriteriaType+MatchingType</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_1_0025</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_1_0026</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_1_0028</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_1_0029</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_1_0030</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_1_0032</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_1_0033</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_1_0034</t>
+  </si>
+  <si>
+    <t>OTLC-1234</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_2_0024</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_2_0025</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_2_0026</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_2_0028</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_2_0029</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_2_0030</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_2_0032</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_2_0033</t>
+  </si>
+  <si>
+    <t>searchOnlineAccounts_2_0034</t>
+  </si>
+  <si>
+    <t>Not a live scenario</t>
+  </si>
+  <si>
+    <t>Prasannanarayanan Gunasekaran</t>
+  </si>
+  <si>
+    <t>Gaurav Rathi</t>
   </si>
 </sst>
 </file>
@@ -418,15 +487,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -440,6 +500,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,10 +817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B41" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42:I49"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,16 +1177,16 @@
       <c r="D14" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="11" t="s">
         <v>51</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="6" t="s">
+      <c r="G14" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="11" t="s">
         <v>28</v>
       </c>
       <c r="I14" s="4"/>
@@ -1135,12 +1204,12 @@
       <c r="D15" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="7"/>
+      <c r="E15" s="12"/>
       <c r="F15" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1156,12 +1225,12 @@
       <c r="D16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="7"/>
+      <c r="E16" s="12"/>
       <c r="F16" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1177,12 +1246,12 @@
       <c r="D17" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="7"/>
+      <c r="E17" s="12"/>
       <c r="F17" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1198,12 +1267,12 @@
       <c r="D18" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E18" s="7"/>
+      <c r="E18" s="12"/>
       <c r="F18" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
       <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1219,12 +1288,12 @@
       <c r="D19" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="7"/>
+      <c r="E19" s="12"/>
       <c r="F19" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1240,12 +1309,12 @@
       <c r="D20" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="7"/>
+      <c r="E20" s="12"/>
       <c r="F20" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
       <c r="I20" s="4"/>
     </row>
     <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1261,12 +1330,12 @@
       <c r="D21" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E21" s="7"/>
+      <c r="E21" s="12"/>
       <c r="F21" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
       <c r="I21" s="4"/>
     </row>
     <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1282,12 +1351,12 @@
       <c r="D22" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="7"/>
+      <c r="E22" s="12"/>
       <c r="F22" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
       <c r="I22" s="4"/>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1303,12 +1372,12 @@
       <c r="D23" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="7"/>
+      <c r="E23" s="12"/>
       <c r="F23" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1324,12 +1393,12 @@
       <c r="D24" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E24" s="7"/>
+      <c r="E24" s="12"/>
       <c r="F24" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1345,12 +1414,12 @@
       <c r="D25" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="7"/>
+      <c r="E25" s="12"/>
       <c r="F25" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1366,12 +1435,12 @@
       <c r="D26" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="7"/>
+      <c r="E26" s="12"/>
       <c r="F26" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
       <c r="I26" s="4"/>
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1387,12 +1456,12 @@
       <c r="D27" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="7"/>
+      <c r="E27" s="12"/>
       <c r="F27" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
       <c r="I27" s="4"/>
     </row>
     <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1408,12 +1477,12 @@
       <c r="D28" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E28" s="7"/>
+      <c r="E28" s="12"/>
       <c r="F28" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
       <c r="I28" s="4"/>
     </row>
     <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1429,12 +1498,12 @@
       <c r="D29" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E29" s="7"/>
+      <c r="E29" s="12"/>
       <c r="F29" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
       <c r="I29" s="4"/>
     </row>
     <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1450,12 +1519,12 @@
       <c r="D30" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E30" s="7"/>
+      <c r="E30" s="12"/>
       <c r="F30" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
       <c r="I30" s="4"/>
     </row>
     <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1471,12 +1540,12 @@
       <c r="D31" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="7"/>
+      <c r="E31" s="12"/>
       <c r="F31" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
       <c r="I31" s="4"/>
     </row>
     <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -1492,12 +1561,12 @@
       <c r="D32" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E32" s="7"/>
+      <c r="E32" s="12"/>
       <c r="F32" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
       <c r="I32" s="4"/>
     </row>
     <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1513,12 +1582,12 @@
       <c r="D33" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E33" s="7"/>
+      <c r="E33" s="12"/>
       <c r="F33" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
       <c r="I33" s="4"/>
     </row>
     <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1534,12 +1603,12 @@
       <c r="D34" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="7"/>
+      <c r="E34" s="12"/>
       <c r="F34" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
       <c r="I34" s="4"/>
     </row>
     <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1555,28 +1624,28 @@
       <c r="D35" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E35" s="8"/>
+      <c r="E35" s="13"/>
       <c r="F35" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="E36" s="12" t="s">
+      <c r="E36" s="9" t="s">
         <v>31</v>
       </c>
       <c r="F36" s="3" t="s">
@@ -1585,23 +1654,25 @@
       <c r="G36" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H36" s="13"/>
-      <c r="I36" s="13"/>
-    </row>
-    <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H36" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I36" s="10"/>
+    </row>
+    <row r="37" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E37" s="9" t="s">
         <v>31</v>
       </c>
       <c r="F37" s="3" t="s">
@@ -1610,23 +1681,25 @@
       <c r="G37" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-    </row>
-    <row r="38" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H37" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I37" s="10"/>
+    </row>
+    <row r="38" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D38" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E38" s="12" t="s">
+      <c r="E38" s="9" t="s">
         <v>31</v>
       </c>
       <c r="F38" s="3" t="s">
@@ -1635,23 +1708,25 @@
       <c r="G38" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-    </row>
-    <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H38" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I38" s="10"/>
+    </row>
+    <row r="39" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D39" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E39" s="12" t="s">
+      <c r="E39" s="9" t="s">
         <v>31</v>
       </c>
       <c r="F39" s="3" t="s">
@@ -1660,23 +1735,25 @@
       <c r="G39" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-    </row>
-    <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H39" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I39" s="10"/>
+    </row>
+    <row r="40" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="D40" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="9" t="s">
         <v>31</v>
       </c>
       <c r="F40" s="3" t="s">
@@ -1685,23 +1762,25 @@
       <c r="G40" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-    </row>
-    <row r="41" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H40" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I40" s="10"/>
+    </row>
+    <row r="41" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D41" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E41" s="12" t="s">
+      <c r="E41" s="9" t="s">
         <v>31</v>
       </c>
       <c r="F41" s="3" t="s">
@@ -1710,23 +1789,25 @@
       <c r="G41" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-    </row>
-    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H41" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I41" s="10"/>
+    </row>
+    <row r="42" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>41</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D42" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="E42" s="12" t="s">
+      <c r="E42" s="9" t="s">
         <v>31</v>
       </c>
       <c r="F42" s="3" t="s">
@@ -1735,23 +1816,25 @@
       <c r="G42" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-    </row>
-    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H42" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I42" s="10"/>
+    </row>
+    <row r="43" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>42</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C43" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D43" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="E43" s="9" t="s">
         <v>31</v>
       </c>
       <c r="F43" s="3" t="s">
@@ -1760,23 +1843,25 @@
       <c r="G43" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H43" s="13"/>
-      <c r="I43" s="13"/>
-    </row>
-    <row r="44" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H43" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I43" s="10"/>
+    </row>
+    <row r="44" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="10" t="s">
+      <c r="C44" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D44" s="9" t="s">
+      <c r="D44" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E44" s="12" t="s">
+      <c r="E44" s="9" t="s">
         <v>31</v>
       </c>
       <c r="F44" s="3" t="s">
@@ -1785,23 +1870,25 @@
       <c r="G44" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
-    </row>
-    <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H44" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I44" s="10"/>
+    </row>
+    <row r="45" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>44</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D45" s="9" t="s">
+      <c r="D45" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E45" s="12" t="s">
+      <c r="E45" s="9" t="s">
         <v>31</v>
       </c>
       <c r="F45" s="3" t="s">
@@ -1810,23 +1897,25 @@
       <c r="G45" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H45" s="13"/>
-      <c r="I45" s="13"/>
-    </row>
-    <row r="46" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H45" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I45" s="10"/>
+    </row>
+    <row r="46" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>45</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="E46" s="9" t="s">
         <v>31</v>
       </c>
       <c r="F46" s="3" t="s">
@@ -1835,23 +1924,25 @@
       <c r="G46" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
-    </row>
-    <row r="47" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H46" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I46" s="10"/>
+    </row>
+    <row r="47" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="D47" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="E47" s="12" t="s">
+      <c r="E47" s="9" t="s">
         <v>31</v>
       </c>
       <c r="F47" s="3" t="s">
@@ -1860,23 +1951,25 @@
       <c r="G47" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
-    </row>
-    <row r="48" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H47" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I47" s="10"/>
+    </row>
+    <row r="48" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>47</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D48" s="12" t="s">
+      <c r="D48" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="E48" s="12" t="s">
+      <c r="E48" s="9" t="s">
         <v>31</v>
       </c>
       <c r="F48" s="3" t="s">
@@ -1885,23 +1978,25 @@
       <c r="G48" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H48" s="13"/>
-      <c r="I48" s="13"/>
-    </row>
-    <row r="49" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="H48" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I48" s="10"/>
+    </row>
+    <row r="49" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="C49" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="D49" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="E49" s="12" t="s">
+      <c r="E49" s="9" t="s">
         <v>31</v>
       </c>
       <c r="F49" s="3" t="s">
@@ -1910,8 +2005,460 @@
       <c r="G49" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
+      <c r="H49" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I49" s="10"/>
+    </row>
+    <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+      <c r="B50" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I50" s="10"/>
+    </row>
+    <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I51" s="10"/>
+    </row>
+    <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+      <c r="B52" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I52" s="10"/>
+    </row>
+    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="4"/>
+      <c r="B53" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I53" s="10"/>
+    </row>
+    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I54" s="10"/>
+    </row>
+    <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G55" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I55" s="10"/>
+    </row>
+    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I56" s="10"/>
+    </row>
+    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I57" s="10"/>
+    </row>
+    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+      <c r="B58" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I58" s="10"/>
+    </row>
+    <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+      <c r="B59" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I59" s="10"/>
+    </row>
+    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I60" s="10"/>
+    </row>
+    <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I61" s="10"/>
+    </row>
+    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A62" s="4"/>
+      <c r="B62" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I62" s="10"/>
+    </row>
+    <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I63" s="10"/>
+    </row>
+    <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I64" s="10"/>
+    </row>
+    <row r="65" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A65" s="4"/>
+      <c r="B65" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I65" s="10"/>
+    </row>
+    <row r="66" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H66" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I66" s="10"/>
+    </row>
+    <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H67" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I67" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
[AS]-Updated REF-INT 3.2 Pack and Change details sheet
</commit_message>
<xml_diff>
--- a/REF-INT 3.2 Change Details.xlsx
+++ b/REF-INT 3.2 Change Details.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="120">
   <si>
     <t>S.No.</t>
   </si>
@@ -369,6 +369,30 @@
   </si>
   <si>
     <t>Gaurav Rathi</t>
+  </si>
+  <si>
+    <t>searchOnlineAccount_2_001</t>
+  </si>
+  <si>
+    <t>searchOnlineAccount_2_003</t>
+  </si>
+  <si>
+    <t>searchOnlineAccount_2_008</t>
+  </si>
+  <si>
+    <t>searchOnlineAccount_2_009</t>
+  </si>
+  <si>
+    <t>searchOnlineAccount_2_053</t>
+  </si>
+  <si>
+    <t>Need to change data</t>
+  </si>
+  <si>
+    <t>We have to change the data</t>
+  </si>
+  <si>
+    <t>Alagesh Ramu/ Nitish Agarwal</t>
   </si>
 </sst>
 </file>
@@ -817,20 +841,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I67"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26.85546875" customWidth="1"/>
-    <col min="3" max="3" width="32.28515625" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" customWidth="1"/>
     <col min="4" max="4" width="30.5703125" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
     <col min="6" max="6" width="61" customWidth="1"/>
     <col min="7" max="7" width="37.7109375" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2011,7 +2036,9 @@
       <c r="I49" s="10"/>
     </row>
     <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
+      <c r="A50" s="4">
+        <v>49</v>
+      </c>
       <c r="B50" s="4" t="s">
         <v>19</v>
       </c>
@@ -2036,7 +2063,9 @@
       <c r="I50" s="10"/>
     </row>
     <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
+      <c r="A51" s="4">
+        <v>50</v>
+      </c>
       <c r="B51" s="4" t="s">
         <v>19</v>
       </c>
@@ -2061,7 +2090,9 @@
       <c r="I51" s="10"/>
     </row>
     <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
+      <c r="A52" s="4">
+        <v>51</v>
+      </c>
       <c r="B52" s="4" t="s">
         <v>19</v>
       </c>
@@ -2086,7 +2117,9 @@
       <c r="I52" s="10"/>
     </row>
     <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
+      <c r="A53" s="4">
+        <v>52</v>
+      </c>
       <c r="B53" s="4" t="s">
         <v>19</v>
       </c>
@@ -2111,7 +2144,9 @@
       <c r="I53" s="10"/>
     </row>
     <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
+      <c r="A54" s="4">
+        <v>53</v>
+      </c>
       <c r="B54" s="4" t="s">
         <v>19</v>
       </c>
@@ -2136,7 +2171,9 @@
       <c r="I54" s="10"/>
     </row>
     <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
+      <c r="A55" s="4">
+        <v>54</v>
+      </c>
       <c r="B55" s="4" t="s">
         <v>19</v>
       </c>
@@ -2161,7 +2198,9 @@
       <c r="I55" s="10"/>
     </row>
     <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
+      <c r="A56" s="4">
+        <v>55</v>
+      </c>
       <c r="B56" s="4" t="s">
         <v>19</v>
       </c>
@@ -2186,7 +2225,9 @@
       <c r="I56" s="10"/>
     </row>
     <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
+      <c r="A57" s="4">
+        <v>56</v>
+      </c>
       <c r="B57" s="4" t="s">
         <v>19</v>
       </c>
@@ -2211,7 +2252,9 @@
       <c r="I57" s="10"/>
     </row>
     <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
+      <c r="A58" s="4">
+        <v>57</v>
+      </c>
       <c r="B58" s="4" t="s">
         <v>19</v>
       </c>
@@ -2236,7 +2279,9 @@
       <c r="I58" s="10"/>
     </row>
     <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
+      <c r="A59" s="4">
+        <v>58</v>
+      </c>
       <c r="B59" s="4" t="s">
         <v>13</v>
       </c>
@@ -2261,7 +2306,9 @@
       <c r="I59" s="10"/>
     </row>
     <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
+      <c r="A60" s="4">
+        <v>59</v>
+      </c>
       <c r="B60" s="4" t="s">
         <v>13</v>
       </c>
@@ -2286,7 +2333,9 @@
       <c r="I60" s="10"/>
     </row>
     <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
+      <c r="A61" s="4">
+        <v>60</v>
+      </c>
       <c r="B61" s="4" t="s">
         <v>13</v>
       </c>
@@ -2311,7 +2360,9 @@
       <c r="I61" s="10"/>
     </row>
     <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
+      <c r="A62" s="4">
+        <v>61</v>
+      </c>
       <c r="B62" s="4" t="s">
         <v>13</v>
       </c>
@@ -2336,7 +2387,9 @@
       <c r="I62" s="10"/>
     </row>
     <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
+      <c r="A63" s="4">
+        <v>62</v>
+      </c>
       <c r="B63" s="4" t="s">
         <v>13</v>
       </c>
@@ -2361,7 +2414,9 @@
       <c r="I63" s="10"/>
     </row>
     <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
+      <c r="A64" s="4">
+        <v>63</v>
+      </c>
       <c r="B64" s="4" t="s">
         <v>13</v>
       </c>
@@ -2386,7 +2441,9 @@
       <c r="I64" s="10"/>
     </row>
     <row r="65" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
+      <c r="A65" s="4">
+        <v>64</v>
+      </c>
       <c r="B65" s="4" t="s">
         <v>13</v>
       </c>
@@ -2411,7 +2468,9 @@
       <c r="I65" s="10"/>
     </row>
     <row r="66" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="4"/>
+      <c r="A66" s="4">
+        <v>65</v>
+      </c>
       <c r="B66" s="4" t="s">
         <v>13</v>
       </c>
@@ -2436,7 +2495,9 @@
       <c r="I66" s="10"/>
     </row>
     <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
+      <c r="A67" s="4">
+        <v>66</v>
+      </c>
       <c r="B67" s="4" t="s">
         <v>13</v>
       </c>
@@ -2459,6 +2520,131 @@
         <v>111</v>
       </c>
       <c r="I67" s="10"/>
+    </row>
+    <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="4">
+        <v>67</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E68" s="9"/>
+      <c r="F68" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H68" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I68" s="10"/>
+    </row>
+    <row r="69" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="4">
+        <v>68</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E69" s="9"/>
+      <c r="F69" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H69" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I69" s="10"/>
+    </row>
+    <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="4">
+        <v>69</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E70" s="9"/>
+      <c r="F70" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H70" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I70" s="10"/>
+    </row>
+    <row r="71" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="4">
+        <v>70</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E71" s="9"/>
+      <c r="F71" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I71" s="10"/>
+    </row>
+    <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A72" s="4">
+        <v>71</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C72" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="E72" s="9"/>
+      <c r="F72" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H72" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I72" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
[AS]-Added test cases for 'Install same MSISDN against multiple PortalIDs' in REF 3.2 pack
</commit_message>
<xml_diff>
--- a/REF-INT 3.2 Change Details.xlsx
+++ b/REF-INT 3.2 Change Details.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="130">
   <si>
     <t>S.No.</t>
   </si>
@@ -393,6 +393,37 @@
   </si>
   <si>
     <t>Alagesh Ramu/ Nitish Agarwal</t>
+  </si>
+  <si>
+    <t>createOnlineAccount_2</t>
+  </si>
+  <si>
+    <t>CreateOnlineAccount_2_Invalid_Values</t>
+  </si>
+  <si>
+    <t>createOnlineAccount_2_WithoutAddress</t>
+  </si>
+  <si>
+    <t>Address fields are not mandatory to pass in the request.</t>
+  </si>
+  <si>
+    <t>We have to change the assertion as without passing address fields we are getting success response.</t>
+  </si>
+  <si>
+    <t>we have same pack for 3.1 and 3.2 so that behavior always remains same, be it any phase. 
+so changing assertion will pass it in 3.2 but fail in 3.1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We have to disable the testcases </t>
+  </si>
+  <si>
+    <t>No change in TestCases</t>
+  </si>
+  <si>
+    <t>As discussed in review meeting on 08/30 it needs some code change, "53/61/71/72/79 -- actual 1 issue (Leagacycustomer search)" so assigning it back to</t>
+  </si>
+  <si>
+    <t>Data Issue</t>
   </si>
 </sst>
 </file>
@@ -514,12 +545,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -532,6 +557,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -841,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,7 +925,7 @@
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -906,18 +937,22 @@
       <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="2"/>
+      <c r="G2" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>128</v>
+      </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -926,19 +961,25 @@
       <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="2"/>
+      <c r="F3" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -950,18 +991,22 @@
       <c r="F4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="3"/>
-      <c r="H4" s="2"/>
+      <c r="G4" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>110</v>
+      </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -973,18 +1018,22 @@
       <c r="F5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="2"/>
+      <c r="G5" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>110</v>
+      </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -996,8 +1045,12 @@
       <c r="F6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="3"/>
-      <c r="H6" s="2"/>
+      <c r="G6" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>110</v>
+      </c>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1007,7 +1060,7 @@
       <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -1034,7 +1087,7 @@
       <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -1054,14 +1107,14 @@
       </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -1081,14 +1134,14 @@
       </c>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -1108,14 +1161,14 @@
       </c>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -1135,14 +1188,14 @@
       </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -1169,7 +1222,7 @@
       <c r="B13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>45</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -1196,22 +1249,22 @@
       <c r="B14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="9" t="s">
         <v>51</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="9" t="s">
         <v>28</v>
       </c>
       <c r="I14" s="4"/>
@@ -1223,18 +1276,18 @@
       <c r="B15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="12"/>
+      <c r="E15" s="10"/>
       <c r="F15" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1244,18 +1297,18 @@
       <c r="B16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="12"/>
+      <c r="E16" s="10"/>
       <c r="F16" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
       <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1265,18 +1318,18 @@
       <c r="B17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="12"/>
+      <c r="E17" s="10"/>
       <c r="F17" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
       <c r="I17" s="4"/>
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1286,18 +1339,18 @@
       <c r="B18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E18" s="12"/>
+      <c r="E18" s="10"/>
       <c r="F18" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
       <c r="I18" s="4"/>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1307,18 +1360,18 @@
       <c r="B19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>62</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="12"/>
+      <c r="E19" s="10"/>
       <c r="F19" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
       <c r="I19" s="4"/>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1328,39 +1381,39 @@
       <c r="B20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="12"/>
+      <c r="E20" s="10"/>
       <c r="F20" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E21" s="12"/>
+      <c r="E21" s="10"/>
       <c r="F21" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
       <c r="I21" s="4"/>
     </row>
     <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1370,18 +1423,18 @@
       <c r="B22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="3" t="s">
         <v>68</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="12"/>
+      <c r="E22" s="10"/>
       <c r="F22" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
       <c r="I22" s="4"/>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1391,18 +1444,18 @@
       <c r="B23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="3" t="s">
         <v>70</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="12"/>
+      <c r="E23" s="10"/>
       <c r="F23" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1412,18 +1465,18 @@
       <c r="B24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E24" s="12"/>
+      <c r="E24" s="10"/>
       <c r="F24" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
       <c r="I24" s="4"/>
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1433,18 +1486,18 @@
       <c r="B25" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="12"/>
+      <c r="E25" s="10"/>
       <c r="F25" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
       <c r="I25" s="4"/>
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1454,18 +1507,18 @@
       <c r="B26" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C26" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E26" s="12"/>
+      <c r="E26" s="10"/>
       <c r="F26" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
       <c r="I26" s="4"/>
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1475,18 +1528,18 @@
       <c r="B27" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E27" s="12"/>
+      <c r="E27" s="10"/>
       <c r="F27" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
       <c r="I27" s="4"/>
     </row>
     <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1496,18 +1549,18 @@
       <c r="B28" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E28" s="12"/>
+      <c r="E28" s="10"/>
       <c r="F28" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
       <c r="I28" s="4"/>
     </row>
     <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1517,18 +1570,18 @@
       <c r="B29" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="E29" s="12"/>
+      <c r="E29" s="10"/>
       <c r="F29" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
       <c r="I29" s="4"/>
     </row>
     <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1538,18 +1591,18 @@
       <c r="B30" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>62</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E30" s="12"/>
+      <c r="E30" s="10"/>
       <c r="F30" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
       <c r="I30" s="4"/>
     </row>
     <row r="31" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1559,39 +1612,39 @@
       <c r="B31" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="3" t="s">
         <v>64</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="12"/>
+      <c r="E31" s="10"/>
       <c r="F31" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
       <c r="I31" s="4"/>
     </row>
-    <row r="32" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>31</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="3" t="s">
         <v>66</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E32" s="12"/>
+      <c r="E32" s="10"/>
       <c r="F32" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
       <c r="I32" s="4"/>
     </row>
     <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1601,18 +1654,18 @@
       <c r="B33" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="3" t="s">
         <v>68</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E33" s="12"/>
+      <c r="E33" s="10"/>
       <c r="F33" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
       <c r="I33" s="4"/>
     </row>
     <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1622,18 +1675,18 @@
       <c r="B34" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="3" t="s">
         <v>70</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E34" s="12"/>
+      <c r="E34" s="10"/>
       <c r="F34" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
       <c r="I34" s="4"/>
     </row>
     <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1643,34 +1696,34 @@
       <c r="B35" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="3" t="s">
         <v>72</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E35" s="13"/>
+      <c r="E35" s="11"/>
       <c r="F35" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>35</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="E36" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F36" s="3" t="s">
@@ -1682,22 +1735,22 @@
       <c r="H36" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="I36" s="10"/>
-    </row>
-    <row r="37" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="I36" s="8"/>
+    </row>
+    <row r="37" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>36</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="D37" s="9" t="s">
+      <c r="D37" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="E37" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F37" s="3" t="s">
@@ -1709,22 +1762,22 @@
       <c r="H37" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="I37" s="10"/>
-    </row>
-    <row r="38" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="I37" s="8"/>
+    </row>
+    <row r="38" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>37</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="D38" s="9" t="s">
+      <c r="D38" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="E38" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F38" s="3" t="s">
@@ -1736,22 +1789,22 @@
       <c r="H38" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="I38" s="10"/>
-    </row>
-    <row r="39" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="I38" s="8"/>
+    </row>
+    <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>38</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D39" s="9" t="s">
+      <c r="D39" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E39" s="9" t="s">
+      <c r="E39" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F39" s="3" t="s">
@@ -1763,22 +1816,22 @@
       <c r="H39" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="I39" s="10"/>
-    </row>
-    <row r="40" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="I39" s="8"/>
+    </row>
+    <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>39</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D40" s="9" t="s">
+      <c r="D40" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E40" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F40" s="3" t="s">
@@ -1790,22 +1843,22 @@
       <c r="H40" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="I40" s="10"/>
-    </row>
-    <row r="41" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="I40" s="8"/>
+    </row>
+    <row r="41" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>40</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="D41" s="9" t="s">
+      <c r="D41" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E41" s="9" t="s">
+      <c r="E41" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F41" s="3" t="s">
@@ -1817,22 +1870,22 @@
       <c r="H41" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="I41" s="10"/>
-    </row>
-    <row r="42" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="I41" s="8"/>
+    </row>
+    <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>41</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="D42" s="9" t="s">
+      <c r="D42" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E42" s="9" t="s">
+      <c r="E42" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F42" s="3" t="s">
@@ -1844,22 +1897,22 @@
       <c r="H42" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="I42" s="10"/>
-    </row>
-    <row r="43" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="I42" s="8"/>
+    </row>
+    <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>42</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="13" t="s">
         <v>75</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E43" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F43" s="3" t="s">
@@ -1871,22 +1924,22 @@
       <c r="H43" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="I43" s="10"/>
-    </row>
-    <row r="44" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="I43" s="8"/>
+    </row>
+    <row r="44" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>43</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="13" t="s">
         <v>62</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E44" s="9" t="s">
+      <c r="E44" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F44" s="3" t="s">
@@ -1898,22 +1951,22 @@
       <c r="H44" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="I44" s="10"/>
-    </row>
-    <row r="45" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="I44" s="8"/>
+    </row>
+    <row r="45" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>44</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="13" t="s">
         <v>64</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="E45" s="9" t="s">
+      <c r="E45" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F45" s="3" t="s">
@@ -1925,22 +1978,22 @@
       <c r="H45" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="I45" s="10"/>
-    </row>
-    <row r="46" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="I45" s="8"/>
+    </row>
+    <row r="46" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>45</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D46" s="9" t="s">
+      <c r="D46" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="E46" s="9" t="s">
+      <c r="E46" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F46" s="3" t="s">
@@ -1952,22 +2005,22 @@
       <c r="H46" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="I46" s="10"/>
-    </row>
-    <row r="47" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="I46" s="8"/>
+    </row>
+    <row r="47" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>46</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D47" s="9" t="s">
+      <c r="D47" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E47" s="9" t="s">
+      <c r="E47" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F47" s="3" t="s">
@@ -1979,22 +2032,22 @@
       <c r="H47" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="I47" s="10"/>
-    </row>
-    <row r="48" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="I47" s="8"/>
+    </row>
+    <row r="48" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>47</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="D48" s="9" t="s">
+      <c r="D48" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E48" s="9" t="s">
+      <c r="E48" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F48" s="3" t="s">
@@ -2006,22 +2059,22 @@
       <c r="H48" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="I48" s="10"/>
-    </row>
-    <row r="49" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="I48" s="8"/>
+    </row>
+    <row r="49" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>48</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C49" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="D49" s="9" t="s">
+      <c r="D49" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E49" s="9" t="s">
+      <c r="E49" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F49" s="3" t="s">
@@ -2033,7 +2086,7 @@
       <c r="H49" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="I49" s="10"/>
+      <c r="I49" s="8"/>
     </row>
     <row r="50" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
@@ -2042,13 +2095,13 @@
       <c r="B50" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C50" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D50" s="9" t="s">
+      <c r="D50" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E50" s="9" t="s">
+      <c r="E50" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F50" s="3" t="s">
@@ -2060,7 +2113,7 @@
       <c r="H50" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I50" s="10"/>
+      <c r="I50" s="8"/>
     </row>
     <row r="51" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
@@ -2069,13 +2122,13 @@
       <c r="B51" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D51" s="9" t="s">
+      <c r="D51" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="E51" s="9" t="s">
+      <c r="E51" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F51" s="3" t="s">
@@ -2087,7 +2140,7 @@
       <c r="H51" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I51" s="10"/>
+      <c r="I51" s="8"/>
     </row>
     <row r="52" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
@@ -2096,13 +2149,13 @@
       <c r="B52" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C52" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D52" s="9" t="s">
+      <c r="D52" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="E52" s="9" t="s">
+      <c r="E52" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F52" s="3" t="s">
@@ -2114,7 +2167,7 @@
       <c r="H52" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I52" s="10"/>
+      <c r="I52" s="8"/>
     </row>
     <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
@@ -2123,13 +2176,13 @@
       <c r="B53" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C53" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="9" t="s">
+      <c r="D53" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="E53" s="9" t="s">
+      <c r="E53" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F53" s="3" t="s">
@@ -2141,7 +2194,7 @@
       <c r="H53" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I53" s="10"/>
+      <c r="I53" s="8"/>
     </row>
     <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
@@ -2150,13 +2203,13 @@
       <c r="B54" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C54" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D54" s="9" t="s">
+      <c r="D54" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E54" s="9" t="s">
+      <c r="E54" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F54" s="3" t="s">
@@ -2168,7 +2221,7 @@
       <c r="H54" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I54" s="10"/>
+      <c r="I54" s="8"/>
     </row>
     <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
@@ -2177,13 +2230,13 @@
       <c r="B55" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D55" s="9" t="s">
+      <c r="D55" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E55" s="9" t="s">
+      <c r="E55" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F55" s="3" t="s">
@@ -2195,7 +2248,7 @@
       <c r="H55" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I55" s="10"/>
+      <c r="I55" s="8"/>
     </row>
     <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
@@ -2204,13 +2257,13 @@
       <c r="B56" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D56" s="9" t="s">
+      <c r="D56" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="E56" s="9" t="s">
+      <c r="E56" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F56" s="3" t="s">
@@ -2222,7 +2275,7 @@
       <c r="H56" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I56" s="10"/>
+      <c r="I56" s="8"/>
     </row>
     <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
@@ -2231,13 +2284,13 @@
       <c r="B57" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D57" s="9" t="s">
+      <c r="D57" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E57" s="9" t="s">
+      <c r="E57" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F57" s="3" t="s">
@@ -2249,7 +2302,7 @@
       <c r="H57" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I57" s="10"/>
+      <c r="I57" s="8"/>
     </row>
     <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
@@ -2258,13 +2311,13 @@
       <c r="B58" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C58" s="8" t="s">
+      <c r="C58" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D58" s="9" t="s">
+      <c r="D58" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E58" s="9" t="s">
+      <c r="E58" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F58" s="3" t="s">
@@ -2276,7 +2329,7 @@
       <c r="H58" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I58" s="10"/>
+      <c r="I58" s="8"/>
     </row>
     <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
@@ -2285,13 +2338,13 @@
       <c r="B59" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C59" s="8" t="s">
+      <c r="C59" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D59" s="9" t="s">
+      <c r="D59" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E59" s="9" t="s">
+      <c r="E59" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F59" s="3" t="s">
@@ -2303,7 +2356,7 @@
       <c r="H59" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I59" s="10"/>
+      <c r="I59" s="8"/>
     </row>
     <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
@@ -2312,13 +2365,13 @@
       <c r="B60" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="C60" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D60" s="9" t="s">
+      <c r="D60" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E60" s="9" t="s">
+      <c r="E60" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F60" s="3" t="s">
@@ -2330,7 +2383,7 @@
       <c r="H60" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I60" s="10"/>
+      <c r="I60" s="8"/>
     </row>
     <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
@@ -2339,13 +2392,13 @@
       <c r="B61" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="C61" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D61" s="9" t="s">
+      <c r="D61" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E61" s="9" t="s">
+      <c r="E61" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F61" s="3" t="s">
@@ -2357,7 +2410,7 @@
       <c r="H61" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I61" s="10"/>
+      <c r="I61" s="8"/>
     </row>
     <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
@@ -2366,13 +2419,13 @@
       <c r="B62" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C62" s="8" t="s">
+      <c r="C62" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D62" s="9" t="s">
+      <c r="D62" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E62" s="9" t="s">
+      <c r="E62" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F62" s="3" t="s">
@@ -2384,7 +2437,7 @@
       <c r="H62" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I62" s="10"/>
+      <c r="I62" s="8"/>
     </row>
     <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
@@ -2393,13 +2446,13 @@
       <c r="B63" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C63" s="8" t="s">
+      <c r="C63" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D63" s="9" t="s">
+      <c r="D63" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E63" s="9" t="s">
+      <c r="E63" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F63" s="3" t="s">
@@ -2411,7 +2464,7 @@
       <c r="H63" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I63" s="10"/>
+      <c r="I63" s="8"/>
     </row>
     <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
@@ -2420,13 +2473,13 @@
       <c r="B64" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C64" s="8" t="s">
+      <c r="C64" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D64" s="9" t="s">
+      <c r="D64" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="E64" s="9" t="s">
+      <c r="E64" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F64" s="3" t="s">
@@ -2438,7 +2491,7 @@
       <c r="H64" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I64" s="10"/>
+      <c r="I64" s="8"/>
     </row>
     <row r="65" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
@@ -2447,13 +2500,13 @@
       <c r="B65" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="C65" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D65" s="9" t="s">
+      <c r="D65" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E65" s="9" t="s">
+      <c r="E65" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F65" s="3" t="s">
@@ -2465,7 +2518,7 @@
       <c r="H65" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I65" s="10"/>
+      <c r="I65" s="8"/>
     </row>
     <row r="66" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
@@ -2474,13 +2527,13 @@
       <c r="B66" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C66" s="8" t="s">
+      <c r="C66" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D66" s="9" t="s">
+      <c r="D66" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="E66" s="9" t="s">
+      <c r="E66" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F66" s="3" t="s">
@@ -2492,7 +2545,7 @@
       <c r="H66" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I66" s="10"/>
+      <c r="I66" s="8"/>
     </row>
     <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
@@ -2501,13 +2554,13 @@
       <c r="B67" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C67" s="8" t="s">
+      <c r="C67" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="D67" s="9" t="s">
+      <c r="D67" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="E67" s="9" t="s">
+      <c r="E67" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F67" s="3" t="s">
@@ -2519,7 +2572,7 @@
       <c r="H67" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I67" s="10"/>
+      <c r="I67" s="8"/>
     </row>
     <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
@@ -2528,13 +2581,15 @@
       <c r="B68" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C68" s="8" t="s">
+      <c r="C68" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D68" s="9" t="s">
+      <c r="D68" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="E68" s="9"/>
+      <c r="E68" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="F68" s="3" t="s">
         <v>117</v>
       </c>
@@ -2544,7 +2599,7 @@
       <c r="H68" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="I68" s="10"/>
+      <c r="I68" s="8"/>
     </row>
     <row r="69" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
@@ -2553,13 +2608,15 @@
       <c r="B69" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C69" s="8" t="s">
+      <c r="C69" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D69" s="9" t="s">
+      <c r="D69" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="E69" s="9"/>
+      <c r="E69" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="F69" s="3" t="s">
         <v>117</v>
       </c>
@@ -2569,7 +2626,7 @@
       <c r="H69" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="I69" s="10"/>
+      <c r="I69" s="8"/>
     </row>
     <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
@@ -2578,13 +2635,15 @@
       <c r="B70" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C70" s="8" t="s">
+      <c r="C70" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D70" s="9" t="s">
+      <c r="D70" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="E70" s="9"/>
+      <c r="E70" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="F70" s="3" t="s">
         <v>117</v>
       </c>
@@ -2594,7 +2653,7 @@
       <c r="H70" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="I70" s="10"/>
+      <c r="I70" s="8"/>
     </row>
     <row r="71" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
@@ -2603,13 +2662,15 @@
       <c r="B71" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C71" s="8" t="s">
+      <c r="C71" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="D71" s="9" t="s">
+      <c r="D71" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E71" s="9"/>
+      <c r="E71" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="F71" s="3" t="s">
         <v>117</v>
       </c>
@@ -2619,7 +2680,7 @@
       <c r="H71" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="I71" s="10"/>
+      <c r="I71" s="8"/>
     </row>
     <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
@@ -2628,13 +2689,15 @@
       <c r="B72" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C72" s="8" t="s">
+      <c r="C72" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="D72" s="9" t="s">
+      <c r="D72" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="E72" s="9"/>
+      <c r="E72" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="F72" s="3" t="s">
         <v>117</v>
       </c>
@@ -2644,7 +2707,30 @@
       <c r="H72" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="I72" s="10"/>
+      <c r="I72" s="8"/>
+    </row>
+    <row r="73" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A73" s="4">
+        <v>72</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C73" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E73" s="7"/>
+      <c r="F73" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H73" s="5"/>
+      <c r="I73" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>